<commit_message>
Updated SQL exports + saving progress
</commit_message>
<xml_diff>
--- a/data/Tables/ID_to_create.xlsx
+++ b/data/Tables/ID_to_create.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/marin_pellan_polymtlus_ca/Documents/Desktop/POST_DOC/Project/canada_metal_sustainability_db/data/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC104887411C794C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6657A51F-6AC9-4FEF-8A7C-318FDB0C5C4A}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC104887411C794C5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD320464-BCB3-434E-B655-786C228DA93A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-20100" yWindow="2280" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">companies!$C$1:$F$329</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="996">
   <si>
     <t>main_id</t>
   </si>
@@ -3007,13 +3008,35 @@
   </si>
   <si>
     <t>facility_group_name</t>
+  </si>
+  <si>
+    <t>Integrated Nickel Operations</t>
+  </si>
+  <si>
+    <t>Contrecoeur</t>
+  </si>
+  <si>
+    <t>AMMC</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>"The raw ore from Fire Lake is sent to our Mont-Wright mining complex where all our ore is crushed, ground and concentrated. Our concentrate is then transported by rail to Port-Cartier, where it will either be sent to our plant to be made into iron oxide pellets or directly to our port to be shipped to international markets.
+The combined production of our Mont-Wright and Fire Lake mines represents over 30% of the ArcelorMittal Group’s global iron ore supply."</t>
+  </si>
+  <si>
+    <t>CCR?</t>
+  </si>
+  <si>
+    <t>"At Horne Smelter, we produce 99.1% pure copper anodes. From their arrival at our Rouyn-Noranda smelter, whether by train or truck, to casting in our anode furnaces, the concentrates and recycled products go through various processing stages before the material can then be processed into cathodes at the CCR Refinery in Montréal-Est."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3035,6 +3058,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3087,7 +3118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3101,6 +3132,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8976,10 +9008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2F5FA7-71F9-49C8-9BC8-0B44C1C55C1D}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9007,7 +9039,9 @@
       <c r="E1" s="4" t="s">
         <v>973</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>992</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -9443,7 +9477,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>887</v>
       </c>
@@ -9457,7 +9491,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>887</v>
       </c>
@@ -9471,7 +9505,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>887</v>
       </c>
@@ -9485,114 +9519,231 @@
         <v>983</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>365</v>
+      </c>
+      <c r="B36" t="s">
+        <v>366</v>
+      </c>
+      <c r="C36" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>365</v>
+      </c>
+      <c r="B37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C37" t="s">
+        <v>369</v>
+      </c>
+      <c r="D37" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>365</v>
+      </c>
+      <c r="B38" t="s">
+        <v>370</v>
+      </c>
+      <c r="C38" t="s">
+        <v>371</v>
+      </c>
+      <c r="D38" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>365</v>
+      </c>
+      <c r="B39" t="s">
+        <v>372</v>
+      </c>
+      <c r="C39" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>365</v>
       </c>
       <c r="B40" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="C40" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+      <c r="D40" t="s">
+        <v>994</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>365</v>
       </c>
       <c r="B41" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="C41" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>365</v>
       </c>
       <c r="B42" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="C42" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+      <c r="D42" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>365</v>
       </c>
       <c r="B43" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="C43" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+      <c r="D43" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>365</v>
       </c>
       <c r="B44" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="C44" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+      <c r="D44" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>365</v>
       </c>
       <c r="B45" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="C45" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+      <c r="D45" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>365</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>378</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>365</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>382</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="D47" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>365</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>384</v>
+        <v>82</v>
       </c>
       <c r="C48" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>365</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>386</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>387</v>
+        <v>85</v>
+      </c>
+      <c r="D49" t="s">
+        <v>991</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>991</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" t="s">
+        <v>991</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>